<commit_message>
Change email host and user
</commit_message>
<xml_diff>
--- a/assets/excel/ea_report.xlsx
+++ b/assets/excel/ea_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C566D0-CDFE-488B-AFFC-2D1DA555B132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1B8AAA-6BA8-4C50-A884-AF4FE6545E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2157,7 +2157,7 @@
   <dimension ref="A1:AP43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2370,10 +2370,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="162"/>
-      <c r="G5" s="117">
-        <f ca="1" xml:space="preserve"> NOW()</f>
-        <v>44703.95222511574</v>
-      </c>
+      <c r="G5" s="117"/>
       <c r="H5" s="162" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Generate TER form by total days of travel
</commit_message>
<xml_diff>
--- a/assets/excel/ea_report.xlsx
+++ b/assets/excel/ea_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50FF1C4-991B-4D3C-AEA6-0FE291157565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D4D8C4-EDBC-4C0F-9D2B-B96CE7A43757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2156,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3455,7 +3455,7 @@
       <c r="B38" s="19"/>
       <c r="C38" s="120"/>
       <c r="D38" s="132">
-        <f>J15+J16+J17+J18+J23+J27+J26+J28</f>
+        <f>J15+J16+J17+J18+J19+J23+J27+J26+J28</f>
         <v>0</v>
       </c>
       <c r="E38" s="87"/>

</xml_diff>

<commit_message>
EA Request excel format for 5 destinations
</commit_message>
<xml_diff>
--- a/assets/excel/ea_report.xlsx
+++ b/assets/excel/ea_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D4D8C4-EDBC-4C0F-9D2B-B96CE7A43757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44C422F-F7AD-4C50-8978-46BB642132B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2157,7 +2157,7 @@
   <dimension ref="A1:AP43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3455,7 +3455,7 @@
       <c r="B38" s="19"/>
       <c r="C38" s="120"/>
       <c r="D38" s="132">
-        <f>J15+J16+J17+J18+J19+J23+J27+J26+J28</f>
+        <f>J15+J16+J17+J18+J19+J23+J27+J26+J28+J24+J25+J29</f>
         <v>0</v>
       </c>
       <c r="E38" s="87"/>
@@ -3494,10 +3494,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="89"/>
-      <c r="D40" s="136">
-        <f>J19+J24+J25+J30+J31</f>
-        <v>0</v>
-      </c>
+      <c r="D40" s="136"/>
       <c r="E40" s="92"/>
       <c r="F40" s="137"/>
       <c r="G40" s="136"/>

</xml_diff>

<commit_message>
Set max travel time to 28 days
</commit_message>
<xml_diff>
--- a/assets/excel/ea_report.xlsx
+++ b/assets/excel/ea_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44C422F-F7AD-4C50-8978-46BB642132B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54AB29B-8705-47B3-8241-100E7C362FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
     <numFmt numFmtId="169" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="170" formatCode="[$-13809]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -688,6 +688,10 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1252,12 +1256,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1616,9 +1621,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="32" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1735,11 +1737,18 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Koma" xfId="2" builtinId="3"/>
     <cellStyle name="Mata Uang" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Persen" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2156,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2174,243 +2183,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="121"/>
-      <c r="Y1" s="121"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="121"/>
-      <c r="AB1" s="121"/>
-      <c r="AC1" s="121"/>
-      <c r="AD1" s="121"/>
-      <c r="AE1" s="121"/>
-      <c r="AF1" s="121"/>
-      <c r="AG1" s="121"/>
-      <c r="AH1" s="121"/>
-      <c r="AI1" s="121"/>
-      <c r="AJ1" s="121"/>
-      <c r="AK1" s="121"/>
-      <c r="AL1" s="121"/>
-      <c r="AM1" s="121"/>
-      <c r="AN1" s="121"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="121"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="120"/>
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="120"/>
+      <c r="AA1" s="120"/>
+      <c r="AB1" s="120"/>
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="120"/>
+      <c r="AF1" s="120"/>
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="120"/>
+      <c r="AI1" s="120"/>
+      <c r="AJ1" s="120"/>
+      <c r="AK1" s="120"/>
+      <c r="AL1" s="120"/>
+      <c r="AM1" s="120"/>
+      <c r="AN1" s="120"/>
+      <c r="AO1" s="120"/>
+      <c r="AP1" s="120"/>
     </row>
     <row r="2" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157"/>
-      <c r="B2" s="159" t="s">
+      <c r="A2" s="156"/>
+      <c r="B2" s="158" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="159"/>
-      <c r="M2" s="159"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="121"/>
-      <c r="Q2" s="121"/>
-      <c r="R2" s="121"/>
-      <c r="S2" s="121"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="121"/>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-      <c r="AI2" s="121"/>
-      <c r="AJ2" s="121"/>
-      <c r="AK2" s="121"/>
-      <c r="AL2" s="121"/>
-      <c r="AM2" s="121"/>
-      <c r="AN2" s="121"/>
-      <c r="AO2" s="121"/>
-      <c r="AP2" s="121"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
+      <c r="W2" s="120"/>
+      <c r="X2" s="120"/>
+      <c r="Y2" s="120"/>
+      <c r="Z2" s="120"/>
+      <c r="AA2" s="120"/>
+      <c r="AB2" s="120"/>
+      <c r="AC2" s="120"/>
+      <c r="AD2" s="120"/>
+      <c r="AE2" s="120"/>
+      <c r="AF2" s="120"/>
+      <c r="AG2" s="120"/>
+      <c r="AH2" s="120"/>
+      <c r="AI2" s="120"/>
+      <c r="AJ2" s="120"/>
+      <c r="AK2" s="120"/>
+      <c r="AL2" s="120"/>
+      <c r="AM2" s="120"/>
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="120"/>
+      <c r="AP2" s="120"/>
     </row>
     <row r="3" spans="1:42" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="157"/>
-      <c r="B3" s="160" t="s">
+      <c r="A3" s="156"/>
+      <c r="B3" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="124"/>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="121"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="121"/>
-      <c r="V3" s="121"/>
-      <c r="W3" s="121"/>
-      <c r="X3" s="121"/>
-      <c r="Y3" s="121"/>
-      <c r="Z3" s="121"/>
-      <c r="AA3" s="121"/>
-      <c r="AB3" s="121"/>
-      <c r="AC3" s="121"/>
-      <c r="AD3" s="121"/>
-      <c r="AE3" s="121"/>
-      <c r="AF3" s="121"/>
-      <c r="AG3" s="121"/>
-      <c r="AH3" s="121"/>
-      <c r="AI3" s="121"/>
-      <c r="AJ3" s="121"/>
-      <c r="AK3" s="121"/>
-      <c r="AL3" s="121"/>
-      <c r="AM3" s="121"/>
-      <c r="AN3" s="121"/>
-      <c r="AO3" s="121"/>
-      <c r="AP3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="120"/>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="120"/>
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
+      <c r="AC3" s="120"/>
+      <c r="AD3" s="120"/>
+      <c r="AE3" s="120"/>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="120"/>
+      <c r="AH3" s="120"/>
+      <c r="AI3" s="120"/>
+      <c r="AJ3" s="120"/>
+      <c r="AK3" s="120"/>
+      <c r="AL3" s="120"/>
+      <c r="AM3" s="120"/>
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="120"/>
+      <c r="AP3" s="120"/>
     </row>
     <row r="4" spans="1:42" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="157"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="121"/>
-      <c r="P4" s="121"/>
-      <c r="Q4" s="121"/>
-      <c r="R4" s="121"/>
-      <c r="S4" s="121"/>
-      <c r="T4" s="121"/>
-      <c r="U4" s="121"/>
-      <c r="V4" s="121"/>
-      <c r="W4" s="121"/>
-      <c r="X4" s="121"/>
-      <c r="Y4" s="121"/>
-      <c r="Z4" s="121"/>
-      <c r="AA4" s="121"/>
-      <c r="AB4" s="121"/>
-      <c r="AC4" s="121"/>
-      <c r="AD4" s="121"/>
-      <c r="AE4" s="121"/>
-      <c r="AF4" s="121"/>
-      <c r="AG4" s="121"/>
-      <c r="AH4" s="121"/>
-      <c r="AI4" s="121"/>
-      <c r="AJ4" s="121"/>
-      <c r="AK4" s="121"/>
-      <c r="AL4" s="121"/>
-      <c r="AM4" s="121"/>
-      <c r="AN4" s="121"/>
-      <c r="AO4" s="121"/>
-      <c r="AP4" s="121"/>
+      <c r="A4" s="156"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="120"/>
+      <c r="R4" s="120"/>
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="120"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="120"/>
+      <c r="AA4" s="120"/>
+      <c r="AB4" s="120"/>
+      <c r="AC4" s="120"/>
+      <c r="AD4" s="120"/>
+      <c r="AE4" s="120"/>
+      <c r="AF4" s="120"/>
+      <c r="AG4" s="120"/>
+      <c r="AH4" s="120"/>
+      <c r="AI4" s="120"/>
+      <c r="AJ4" s="120"/>
+      <c r="AK4" s="120"/>
+      <c r="AL4" s="120"/>
+      <c r="AM4" s="120"/>
+      <c r="AN4" s="120"/>
+      <c r="AO4" s="120"/>
+      <c r="AP4" s="120"/>
     </row>
     <row r="5" spans="1:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="161" t="s">
+      <c r="B5" s="160" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="162" t="s">
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="162"/>
+      <c r="F5" s="161"/>
       <c r="G5" s="117"/>
-      <c r="H5" s="162" t="s">
+      <c r="H5" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="162"/>
-      <c r="J5" s="162"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
       <c r="K5" s="114"/>
       <c r="L5" s="37"/>
       <c r="M5" s="5"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="121"/>
-      <c r="P5" s="121"/>
-      <c r="Q5" s="121"/>
-      <c r="R5" s="121"/>
-      <c r="S5" s="121"/>
-      <c r="T5" s="121"/>
-      <c r="U5" s="121"/>
-      <c r="V5" s="121"/>
-      <c r="W5" s="121"/>
-      <c r="X5" s="121"/>
-      <c r="Y5" s="121"/>
-      <c r="Z5" s="121"/>
-      <c r="AA5" s="121"/>
-      <c r="AB5" s="121"/>
-      <c r="AC5" s="121"/>
-      <c r="AD5" s="121"/>
-      <c r="AE5" s="121"/>
-      <c r="AF5" s="121"/>
-      <c r="AG5" s="121"/>
-      <c r="AH5" s="121"/>
-      <c r="AI5" s="121"/>
-      <c r="AJ5" s="121"/>
-      <c r="AK5" s="121"/>
-      <c r="AL5" s="121"/>
-      <c r="AM5" s="121"/>
-      <c r="AN5" s="121"/>
-      <c r="AO5" s="121"/>
-      <c r="AP5" s="121"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="120"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="120"/>
+      <c r="Y5" s="120"/>
+      <c r="Z5" s="120"/>
+      <c r="AA5" s="120"/>
+      <c r="AB5" s="120"/>
+      <c r="AC5" s="120"/>
+      <c r="AD5" s="120"/>
+      <c r="AE5" s="120"/>
+      <c r="AF5" s="120"/>
+      <c r="AG5" s="120"/>
+      <c r="AH5" s="120"/>
+      <c r="AI5" s="120"/>
+      <c r="AJ5" s="120"/>
+      <c r="AK5" s="120"/>
+      <c r="AL5" s="120"/>
+      <c r="AM5" s="120"/>
+      <c r="AN5" s="120"/>
+      <c r="AO5" s="120"/>
+      <c r="AP5" s="120"/>
     </row>
     <row r="6" spans="1:42" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="126"/>
+      <c r="A6" s="125"/>
       <c r="B6" s="8"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
@@ -2424,37 +2433,37 @@
       <c r="L6" s="38"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
-      <c r="O6" s="121"/>
-      <c r="P6" s="121"/>
-      <c r="Q6" s="121"/>
-      <c r="R6" s="121"/>
-      <c r="S6" s="121"/>
-      <c r="T6" s="121"/>
-      <c r="U6" s="121"/>
-      <c r="V6" s="121"/>
-      <c r="W6" s="121"/>
-      <c r="X6" s="121"/>
-      <c r="Y6" s="121"/>
-      <c r="Z6" s="121"/>
-      <c r="AA6" s="121"/>
-      <c r="AB6" s="121"/>
-      <c r="AC6" s="121"/>
-      <c r="AD6" s="121"/>
-      <c r="AE6" s="121"/>
-      <c r="AF6" s="121"/>
-      <c r="AG6" s="121"/>
-      <c r="AH6" s="121"/>
-      <c r="AI6" s="121"/>
-      <c r="AJ6" s="121"/>
-      <c r="AK6" s="121"/>
-      <c r="AL6" s="121"/>
-      <c r="AM6" s="121"/>
-      <c r="AN6" s="121"/>
-      <c r="AO6" s="121"/>
-      <c r="AP6" s="121"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="120"/>
+      <c r="X6" s="120"/>
+      <c r="Y6" s="120"/>
+      <c r="Z6" s="120"/>
+      <c r="AA6" s="120"/>
+      <c r="AB6" s="120"/>
+      <c r="AC6" s="120"/>
+      <c r="AD6" s="120"/>
+      <c r="AE6" s="120"/>
+      <c r="AF6" s="120"/>
+      <c r="AG6" s="120"/>
+      <c r="AH6" s="120"/>
+      <c r="AI6" s="120"/>
+      <c r="AJ6" s="120"/>
+      <c r="AK6" s="120"/>
+      <c r="AL6" s="120"/>
+      <c r="AM6" s="120"/>
+      <c r="AN6" s="120"/>
+      <c r="AO6" s="120"/>
+      <c r="AP6" s="120"/>
     </row>
     <row r="7" spans="1:42" s="112" customFormat="1" ht="33.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="127"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="108"/>
       <c r="C7" s="52" t="s">
         <v>7</v>
@@ -2489,38 +2498,38 @@
       <c r="M7" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="128"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="128"/>
-      <c r="R7" s="128"/>
-      <c r="S7" s="128"/>
-      <c r="T7" s="128"/>
-      <c r="U7" s="128"/>
-      <c r="V7" s="128"/>
-      <c r="W7" s="128"/>
-      <c r="X7" s="128"/>
-      <c r="Y7" s="128"/>
-      <c r="Z7" s="128"/>
-      <c r="AA7" s="128"/>
-      <c r="AB7" s="128"/>
-      <c r="AC7" s="128"/>
-      <c r="AD7" s="128"/>
-      <c r="AE7" s="128"/>
-      <c r="AF7" s="128"/>
-      <c r="AG7" s="128"/>
-      <c r="AH7" s="128"/>
-      <c r="AI7" s="128"/>
-      <c r="AJ7" s="128"/>
-      <c r="AK7" s="128"/>
-      <c r="AL7" s="128"/>
-      <c r="AM7" s="128"/>
-      <c r="AN7" s="128"/>
-      <c r="AO7" s="128"/>
-      <c r="AP7" s="128"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="127"/>
+      <c r="P7" s="127"/>
+      <c r="Q7" s="127"/>
+      <c r="R7" s="127"/>
+      <c r="S7" s="127"/>
+      <c r="T7" s="127"/>
+      <c r="U7" s="127"/>
+      <c r="V7" s="127"/>
+      <c r="W7" s="127"/>
+      <c r="X7" s="127"/>
+      <c r="Y7" s="127"/>
+      <c r="Z7" s="127"/>
+      <c r="AA7" s="127"/>
+      <c r="AB7" s="127"/>
+      <c r="AC7" s="127"/>
+      <c r="AD7" s="127"/>
+      <c r="AE7" s="127"/>
+      <c r="AF7" s="127"/>
+      <c r="AG7" s="127"/>
+      <c r="AH7" s="127"/>
+      <c r="AI7" s="127"/>
+      <c r="AJ7" s="127"/>
+      <c r="AK7" s="127"/>
+      <c r="AL7" s="127"/>
+      <c r="AM7" s="127"/>
+      <c r="AN7" s="127"/>
+      <c r="AO7" s="127"/>
+      <c r="AP7" s="127"/>
     </row>
     <row r="8" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="31" t="s">
         <v>18</v>
       </c>
@@ -2535,35 +2544,35 @@
       <c r="K8" s="56"/>
       <c r="L8" s="39"/>
       <c r="M8" s="104"/>
-      <c r="N8" s="148"/>
-      <c r="O8" s="121"/>
-      <c r="P8" s="121"/>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="121"/>
-      <c r="T8" s="121"/>
-      <c r="U8" s="121"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="121"/>
-      <c r="X8" s="121"/>
-      <c r="Y8" s="121"/>
-      <c r="Z8" s="121"/>
-      <c r="AA8" s="121"/>
-      <c r="AB8" s="121"/>
-      <c r="AC8" s="121"/>
-      <c r="AD8" s="121"/>
-      <c r="AE8" s="121"/>
-      <c r="AF8" s="121"/>
-      <c r="AG8" s="121"/>
-      <c r="AH8" s="121"/>
-      <c r="AI8" s="121"/>
-      <c r="AJ8" s="121"/>
-      <c r="AK8" s="121"/>
-      <c r="AL8" s="121"/>
-      <c r="AM8" s="121"/>
-      <c r="AN8" s="121"/>
-      <c r="AO8" s="121"/>
-      <c r="AP8" s="121"/>
+      <c r="N8" s="147"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="120"/>
+      <c r="Q8" s="120"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
+      <c r="T8" s="120"/>
+      <c r="U8" s="120"/>
+      <c r="V8" s="120"/>
+      <c r="W8" s="120"/>
+      <c r="X8" s="120"/>
+      <c r="Y8" s="120"/>
+      <c r="Z8" s="120"/>
+      <c r="AA8" s="120"/>
+      <c r="AB8" s="120"/>
+      <c r="AC8" s="120"/>
+      <c r="AD8" s="120"/>
+      <c r="AE8" s="120"/>
+      <c r="AF8" s="120"/>
+      <c r="AG8" s="120"/>
+      <c r="AH8" s="120"/>
+      <c r="AI8" s="120"/>
+      <c r="AJ8" s="120"/>
+      <c r="AK8" s="120"/>
+      <c r="AL8" s="120"/>
+      <c r="AM8" s="120"/>
+      <c r="AN8" s="120"/>
+      <c r="AO8" s="120"/>
+      <c r="AP8" s="120"/>
     </row>
     <row r="9" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -2584,34 +2593,34 @@
       <c r="L9" s="40"/>
       <c r="M9" s="22"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="121"/>
-      <c r="T9" s="121"/>
-      <c r="U9" s="121"/>
-      <c r="V9" s="121"/>
-      <c r="W9" s="121"/>
-      <c r="X9" s="121"/>
-      <c r="Y9" s="121"/>
-      <c r="Z9" s="121"/>
-      <c r="AA9" s="121"/>
-      <c r="AB9" s="121"/>
-      <c r="AC9" s="121"/>
-      <c r="AD9" s="121"/>
-      <c r="AE9" s="121"/>
-      <c r="AF9" s="121"/>
-      <c r="AG9" s="121"/>
-      <c r="AH9" s="121"/>
-      <c r="AI9" s="121"/>
-      <c r="AJ9" s="121"/>
-      <c r="AK9" s="121"/>
-      <c r="AL9" s="121"/>
-      <c r="AM9" s="121"/>
-      <c r="AN9" s="121"/>
-      <c r="AO9" s="121"/>
-      <c r="AP9" s="121"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="120"/>
+      <c r="Q9" s="120"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="120"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="120"/>
+      <c r="V9" s="120"/>
+      <c r="W9" s="120"/>
+      <c r="X9" s="120"/>
+      <c r="Y9" s="120"/>
+      <c r="Z9" s="120"/>
+      <c r="AA9" s="120"/>
+      <c r="AB9" s="120"/>
+      <c r="AC9" s="120"/>
+      <c r="AD9" s="120"/>
+      <c r="AE9" s="120"/>
+      <c r="AF9" s="120"/>
+      <c r="AG9" s="120"/>
+      <c r="AH9" s="120"/>
+      <c r="AI9" s="120"/>
+      <c r="AJ9" s="120"/>
+      <c r="AK9" s="120"/>
+      <c r="AL9" s="120"/>
+      <c r="AM9" s="120"/>
+      <c r="AN9" s="120"/>
+      <c r="AO9" s="120"/>
+      <c r="AP9" s="120"/>
     </row>
     <row r="10" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
@@ -2632,34 +2641,34 @@
       <c r="L10" s="41"/>
       <c r="M10" s="22"/>
       <c r="N10" s="12"/>
-      <c r="O10" s="121"/>
-      <c r="P10" s="121"/>
-      <c r="Q10" s="121"/>
-      <c r="R10" s="121"/>
-      <c r="S10" s="121"/>
-      <c r="T10" s="121"/>
-      <c r="U10" s="121"/>
-      <c r="V10" s="121"/>
-      <c r="W10" s="121"/>
-      <c r="X10" s="121"/>
-      <c r="Y10" s="121"/>
-      <c r="Z10" s="121"/>
-      <c r="AA10" s="121"/>
-      <c r="AB10" s="121"/>
-      <c r="AC10" s="121"/>
-      <c r="AD10" s="121"/>
-      <c r="AE10" s="121"/>
-      <c r="AF10" s="121"/>
-      <c r="AG10" s="121"/>
-      <c r="AH10" s="121"/>
-      <c r="AI10" s="121"/>
-      <c r="AJ10" s="121"/>
-      <c r="AK10" s="121"/>
-      <c r="AL10" s="121"/>
-      <c r="AM10" s="121"/>
-      <c r="AN10" s="121"/>
-      <c r="AO10" s="121"/>
-      <c r="AP10" s="121"/>
+      <c r="O10" s="120"/>
+      <c r="P10" s="120"/>
+      <c r="Q10" s="120"/>
+      <c r="R10" s="120"/>
+      <c r="S10" s="120"/>
+      <c r="T10" s="120"/>
+      <c r="U10" s="120"/>
+      <c r="V10" s="120"/>
+      <c r="W10" s="120"/>
+      <c r="X10" s="120"/>
+      <c r="Y10" s="120"/>
+      <c r="Z10" s="120"/>
+      <c r="AA10" s="120"/>
+      <c r="AB10" s="120"/>
+      <c r="AC10" s="120"/>
+      <c r="AD10" s="120"/>
+      <c r="AE10" s="120"/>
+      <c r="AF10" s="120"/>
+      <c r="AG10" s="120"/>
+      <c r="AH10" s="120"/>
+      <c r="AI10" s="120"/>
+      <c r="AJ10" s="120"/>
+      <c r="AK10" s="120"/>
+      <c r="AL10" s="120"/>
+      <c r="AM10" s="120"/>
+      <c r="AN10" s="120"/>
+      <c r="AO10" s="120"/>
+      <c r="AP10" s="120"/>
     </row>
     <row r="11" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
@@ -2680,34 +2689,34 @@
       <c r="L11" s="41"/>
       <c r="M11" s="22"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="121"/>
-      <c r="P11" s="121"/>
-      <c r="Q11" s="121"/>
-      <c r="R11" s="121"/>
-      <c r="S11" s="121"/>
-      <c r="T11" s="121"/>
-      <c r="U11" s="121"/>
-      <c r="V11" s="121"/>
-      <c r="W11" s="121"/>
-      <c r="X11" s="121"/>
-      <c r="Y11" s="121"/>
-      <c r="Z11" s="121"/>
-      <c r="AA11" s="121"/>
-      <c r="AB11" s="121"/>
-      <c r="AC11" s="121"/>
-      <c r="AD11" s="121"/>
-      <c r="AE11" s="121"/>
-      <c r="AF11" s="121"/>
-      <c r="AG11" s="121"/>
-      <c r="AH11" s="121"/>
-      <c r="AI11" s="121"/>
-      <c r="AJ11" s="121"/>
-      <c r="AK11" s="121"/>
-      <c r="AL11" s="121"/>
-      <c r="AM11" s="121"/>
-      <c r="AN11" s="121"/>
-      <c r="AO11" s="121"/>
-      <c r="AP11" s="121"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="120"/>
+      <c r="Q11" s="120"/>
+      <c r="R11" s="120"/>
+      <c r="S11" s="120"/>
+      <c r="T11" s="120"/>
+      <c r="U11" s="120"/>
+      <c r="V11" s="120"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="120"/>
+      <c r="AA11" s="120"/>
+      <c r="AB11" s="120"/>
+      <c r="AC11" s="120"/>
+      <c r="AD11" s="120"/>
+      <c r="AE11" s="120"/>
+      <c r="AF11" s="120"/>
+      <c r="AG11" s="120"/>
+      <c r="AH11" s="120"/>
+      <c r="AI11" s="120"/>
+      <c r="AJ11" s="120"/>
+      <c r="AK11" s="120"/>
+      <c r="AL11" s="120"/>
+      <c r="AM11" s="120"/>
+      <c r="AN11" s="120"/>
+      <c r="AO11" s="120"/>
+      <c r="AP11" s="120"/>
     </row>
     <row r="12" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
@@ -2726,34 +2735,34 @@
       <c r="L12" s="41"/>
       <c r="M12" s="22"/>
       <c r="N12" s="12"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="121"/>
-      <c r="Q12" s="121"/>
-      <c r="R12" s="121"/>
-      <c r="S12" s="121"/>
-      <c r="T12" s="121"/>
-      <c r="U12" s="121"/>
-      <c r="V12" s="121"/>
-      <c r="W12" s="121"/>
-      <c r="X12" s="121"/>
-      <c r="Y12" s="121"/>
-      <c r="Z12" s="121"/>
-      <c r="AA12" s="121"/>
-      <c r="AB12" s="121"/>
-      <c r="AC12" s="121"/>
-      <c r="AD12" s="121"/>
-      <c r="AE12" s="121"/>
-      <c r="AF12" s="121"/>
-      <c r="AG12" s="121"/>
-      <c r="AH12" s="121"/>
-      <c r="AI12" s="121"/>
-      <c r="AJ12" s="121"/>
-      <c r="AK12" s="121"/>
-      <c r="AL12" s="121"/>
-      <c r="AM12" s="121"/>
-      <c r="AN12" s="121"/>
-      <c r="AO12" s="121"/>
-      <c r="AP12" s="121"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="120"/>
+      <c r="W12" s="120"/>
+      <c r="X12" s="120"/>
+      <c r="Y12" s="120"/>
+      <c r="Z12" s="120"/>
+      <c r="AA12" s="120"/>
+      <c r="AB12" s="120"/>
+      <c r="AC12" s="120"/>
+      <c r="AD12" s="120"/>
+      <c r="AE12" s="120"/>
+      <c r="AF12" s="120"/>
+      <c r="AG12" s="120"/>
+      <c r="AH12" s="120"/>
+      <c r="AI12" s="120"/>
+      <c r="AJ12" s="120"/>
+      <c r="AK12" s="120"/>
+      <c r="AL12" s="120"/>
+      <c r="AM12" s="120"/>
+      <c r="AN12" s="120"/>
+      <c r="AO12" s="120"/>
+      <c r="AP12" s="120"/>
     </row>
     <row r="13" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
@@ -2772,34 +2781,34 @@
       <c r="L13" s="41"/>
       <c r="M13" s="22"/>
       <c r="N13" s="12"/>
-      <c r="O13" s="121"/>
-      <c r="P13" s="121"/>
-      <c r="Q13" s="121"/>
-      <c r="R13" s="121"/>
-      <c r="S13" s="121"/>
-      <c r="T13" s="121"/>
-      <c r="U13" s="121"/>
-      <c r="V13" s="121"/>
-      <c r="W13" s="121"/>
-      <c r="X13" s="121"/>
-      <c r="Y13" s="121"/>
-      <c r="Z13" s="121"/>
-      <c r="AA13" s="121"/>
-      <c r="AB13" s="121"/>
-      <c r="AC13" s="121"/>
-      <c r="AD13" s="121"/>
-      <c r="AE13" s="121"/>
-      <c r="AF13" s="121"/>
-      <c r="AG13" s="121"/>
-      <c r="AH13" s="121"/>
-      <c r="AI13" s="121"/>
-      <c r="AJ13" s="121"/>
-      <c r="AK13" s="121"/>
-      <c r="AL13" s="121"/>
-      <c r="AM13" s="121"/>
-      <c r="AN13" s="121"/>
-      <c r="AO13" s="121"/>
-      <c r="AP13" s="121"/>
+      <c r="O13" s="120"/>
+      <c r="P13" s="120"/>
+      <c r="Q13" s="120"/>
+      <c r="R13" s="120"/>
+      <c r="S13" s="120"/>
+      <c r="T13" s="120"/>
+      <c r="U13" s="120"/>
+      <c r="V13" s="120"/>
+      <c r="W13" s="120"/>
+      <c r="X13" s="120"/>
+      <c r="Y13" s="120"/>
+      <c r="Z13" s="120"/>
+      <c r="AA13" s="120"/>
+      <c r="AB13" s="120"/>
+      <c r="AC13" s="120"/>
+      <c r="AD13" s="120"/>
+      <c r="AE13" s="120"/>
+      <c r="AF13" s="120"/>
+      <c r="AG13" s="120"/>
+      <c r="AH13" s="120"/>
+      <c r="AI13" s="120"/>
+      <c r="AJ13" s="120"/>
+      <c r="AK13" s="120"/>
+      <c r="AL13" s="120"/>
+      <c r="AM13" s="120"/>
+      <c r="AN13" s="120"/>
+      <c r="AO13" s="120"/>
+      <c r="AP13" s="120"/>
     </row>
     <row r="14" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
@@ -2818,34 +2827,34 @@
       <c r="L14" s="41"/>
       <c r="M14" s="22"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="121"/>
-      <c r="P14" s="121"/>
-      <c r="Q14" s="121"/>
-      <c r="R14" s="121"/>
-      <c r="S14" s="121"/>
-      <c r="T14" s="121"/>
-      <c r="U14" s="121"/>
-      <c r="V14" s="121"/>
-      <c r="W14" s="121"/>
-      <c r="X14" s="121"/>
-      <c r="Y14" s="121"/>
-      <c r="Z14" s="121"/>
-      <c r="AA14" s="121"/>
-      <c r="AB14" s="121"/>
-      <c r="AC14" s="121"/>
-      <c r="AD14" s="121"/>
-      <c r="AE14" s="121"/>
-      <c r="AF14" s="121"/>
-      <c r="AG14" s="121"/>
-      <c r="AH14" s="121"/>
-      <c r="AI14" s="121"/>
-      <c r="AJ14" s="121"/>
-      <c r="AK14" s="121"/>
-      <c r="AL14" s="121"/>
-      <c r="AM14" s="121"/>
-      <c r="AN14" s="121"/>
-      <c r="AO14" s="121"/>
-      <c r="AP14" s="121"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="120"/>
+      <c r="R14" s="120"/>
+      <c r="S14" s="120"/>
+      <c r="T14" s="120"/>
+      <c r="U14" s="120"/>
+      <c r="V14" s="120"/>
+      <c r="W14" s="120"/>
+      <c r="X14" s="120"/>
+      <c r="Y14" s="120"/>
+      <c r="Z14" s="120"/>
+      <c r="AA14" s="120"/>
+      <c r="AB14" s="120"/>
+      <c r="AC14" s="120"/>
+      <c r="AD14" s="120"/>
+      <c r="AE14" s="120"/>
+      <c r="AF14" s="120"/>
+      <c r="AG14" s="120"/>
+      <c r="AH14" s="120"/>
+      <c r="AI14" s="120"/>
+      <c r="AJ14" s="120"/>
+      <c r="AK14" s="120"/>
+      <c r="AL14" s="120"/>
+      <c r="AM14" s="120"/>
+      <c r="AN14" s="120"/>
+      <c r="AO14" s="120"/>
+      <c r="AP14" s="120"/>
     </row>
     <row r="15" spans="1:42" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2869,34 +2878,34 @@
       <c r="L15" s="42"/>
       <c r="M15" s="22"/>
       <c r="N15" s="13"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="121"/>
-      <c r="Q15" s="121"/>
-      <c r="R15" s="121"/>
-      <c r="S15" s="121"/>
-      <c r="T15" s="121"/>
-      <c r="U15" s="121"/>
-      <c r="V15" s="121"/>
-      <c r="W15" s="121"/>
-      <c r="X15" s="121"/>
-      <c r="Y15" s="121"/>
-      <c r="Z15" s="121"/>
-      <c r="AA15" s="121"/>
-      <c r="AB15" s="121"/>
-      <c r="AC15" s="121"/>
-      <c r="AD15" s="121"/>
-      <c r="AE15" s="121"/>
-      <c r="AF15" s="121"/>
-      <c r="AG15" s="121"/>
-      <c r="AH15" s="121"/>
-      <c r="AI15" s="121"/>
-      <c r="AJ15" s="121"/>
-      <c r="AK15" s="121"/>
-      <c r="AL15" s="121"/>
-      <c r="AM15" s="121"/>
-      <c r="AN15" s="121"/>
-      <c r="AO15" s="121"/>
-      <c r="AP15" s="121"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="120"/>
+      <c r="Q15" s="120"/>
+      <c r="R15" s="120"/>
+      <c r="S15" s="120"/>
+      <c r="T15" s="120"/>
+      <c r="U15" s="120"/>
+      <c r="V15" s="120"/>
+      <c r="W15" s="120"/>
+      <c r="X15" s="120"/>
+      <c r="Y15" s="120"/>
+      <c r="Z15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="120"/>
+      <c r="AC15" s="120"/>
+      <c r="AD15" s="120"/>
+      <c r="AE15" s="120"/>
+      <c r="AF15" s="120"/>
+      <c r="AG15" s="120"/>
+      <c r="AH15" s="120"/>
+      <c r="AI15" s="120"/>
+      <c r="AJ15" s="120"/>
+      <c r="AK15" s="120"/>
+      <c r="AL15" s="120"/>
+      <c r="AM15" s="120"/>
+      <c r="AN15" s="120"/>
+      <c r="AO15" s="120"/>
+      <c r="AP15" s="120"/>
     </row>
     <row r="16" spans="1:42" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -2920,34 +2929,34 @@
       <c r="L16" s="42"/>
       <c r="M16" s="22"/>
       <c r="N16" s="13"/>
-      <c r="O16" s="121"/>
-      <c r="P16" s="121"/>
-      <c r="Q16" s="121"/>
-      <c r="R16" s="121"/>
-      <c r="S16" s="121"/>
-      <c r="T16" s="121"/>
-      <c r="U16" s="121"/>
-      <c r="V16" s="121"/>
-      <c r="W16" s="121"/>
-      <c r="X16" s="121"/>
-      <c r="Y16" s="121"/>
-      <c r="Z16" s="121"/>
-      <c r="AA16" s="121"/>
-      <c r="AB16" s="121"/>
-      <c r="AC16" s="121"/>
-      <c r="AD16" s="121"/>
-      <c r="AE16" s="121"/>
-      <c r="AF16" s="121"/>
-      <c r="AG16" s="121"/>
-      <c r="AH16" s="121"/>
-      <c r="AI16" s="121"/>
-      <c r="AJ16" s="121"/>
-      <c r="AK16" s="121"/>
-      <c r="AL16" s="121"/>
-      <c r="AM16" s="121"/>
-      <c r="AN16" s="121"/>
-      <c r="AO16" s="121"/>
-      <c r="AP16" s="121"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="120"/>
+      <c r="R16" s="120"/>
+      <c r="S16" s="120"/>
+      <c r="T16" s="120"/>
+      <c r="U16" s="120"/>
+      <c r="V16" s="120"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
+      <c r="Y16" s="120"/>
+      <c r="Z16" s="120"/>
+      <c r="AA16" s="120"/>
+      <c r="AB16" s="120"/>
+      <c r="AC16" s="120"/>
+      <c r="AD16" s="120"/>
+      <c r="AE16" s="120"/>
+      <c r="AF16" s="120"/>
+      <c r="AG16" s="120"/>
+      <c r="AH16" s="120"/>
+      <c r="AI16" s="120"/>
+      <c r="AJ16" s="120"/>
+      <c r="AK16" s="120"/>
+      <c r="AL16" s="120"/>
+      <c r="AM16" s="120"/>
+      <c r="AN16" s="120"/>
+      <c r="AO16" s="120"/>
+      <c r="AP16" s="120"/>
     </row>
     <row r="17" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
@@ -2971,7 +2980,7 @@
       <c r="L17" s="42"/>
       <c r="M17" s="22"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="121"/>
+      <c r="O17" s="120"/>
     </row>
     <row r="18" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2995,7 +3004,7 @@
       <c r="L18" s="42"/>
       <c r="M18" s="22"/>
       <c r="N18" s="14"/>
-      <c r="O18" s="121"/>
+      <c r="O18" s="120"/>
     </row>
     <row r="19" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
@@ -3019,7 +3028,7 @@
       <c r="L19" s="42"/>
       <c r="M19" s="22"/>
       <c r="N19" s="14"/>
-      <c r="O19" s="121"/>
+      <c r="O19" s="120"/>
     </row>
     <row r="20" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
@@ -3040,10 +3049,10 @@
         <v>0</v>
       </c>
       <c r="K20" s="67"/>
-      <c r="L20" s="119"/>
+      <c r="L20" s="162"/>
       <c r="M20" s="22"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="129"/>
+      <c r="O20" s="128"/>
     </row>
     <row r="21" spans="1:15" s="7" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -3067,7 +3076,7 @@
       <c r="L21" s="42"/>
       <c r="M21" s="22"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="126"/>
+      <c r="O21" s="125"/>
     </row>
     <row r="22" spans="1:15" s="7" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
@@ -3089,7 +3098,7 @@
       <c r="L22" s="42"/>
       <c r="M22" s="22"/>
       <c r="N22" s="14"/>
-      <c r="O22" s="126"/>
+      <c r="O22" s="125"/>
     </row>
     <row r="23" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
@@ -3113,7 +3122,7 @@
       <c r="L23" s="42"/>
       <c r="M23" s="22"/>
       <c r="N23" s="14"/>
-      <c r="O23" s="121"/>
+      <c r="O23" s="120"/>
     </row>
     <row r="24" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
@@ -3137,7 +3146,7 @@
       <c r="L24" s="42"/>
       <c r="M24" s="22"/>
       <c r="N24" s="14"/>
-      <c r="O24" s="121"/>
+      <c r="O24" s="120"/>
     </row>
     <row r="25" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -3161,7 +3170,7 @@
       <c r="L25" s="42"/>
       <c r="M25" s="22"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="121"/>
+      <c r="O25" s="120"/>
     </row>
     <row r="26" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -3185,7 +3194,7 @@
       <c r="L26" s="42"/>
       <c r="M26" s="22"/>
       <c r="N26" s="14"/>
-      <c r="O26" s="121"/>
+      <c r="O26" s="120"/>
     </row>
     <row r="27" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
@@ -3197,7 +3206,7 @@
       <c r="C27" s="61"/>
       <c r="D27" s="58"/>
       <c r="E27" s="58"/>
-      <c r="F27" s="130"/>
+      <c r="F27" s="129"/>
       <c r="G27" s="68"/>
       <c r="H27" s="61"/>
       <c r="I27" s="58"/>
@@ -3209,7 +3218,7 @@
       <c r="L27" s="118"/>
       <c r="M27" s="22"/>
       <c r="N27" s="14"/>
-      <c r="O27" s="121"/>
+      <c r="O27" s="120"/>
     </row>
     <row r="28" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
@@ -3231,7 +3240,7 @@
       <c r="L28" s="42"/>
       <c r="M28" s="22"/>
       <c r="N28" s="14"/>
-      <c r="O28" s="121"/>
+      <c r="O28" s="120"/>
     </row>
     <row r="29" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
@@ -3255,7 +3264,7 @@
       <c r="L29" s="42"/>
       <c r="M29" s="22"/>
       <c r="N29" s="14"/>
-      <c r="O29" s="121"/>
+      <c r="O29" s="120"/>
     </row>
     <row r="30" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
@@ -3277,7 +3286,7 @@
       <c r="L30" s="42"/>
       <c r="M30" s="22"/>
       <c r="N30" s="14"/>
-      <c r="O30" s="121"/>
+      <c r="O30" s="120"/>
     </row>
     <row r="31" spans="1:15" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
@@ -3299,7 +3308,7 @@
       <c r="L31" s="43"/>
       <c r="M31" s="105"/>
       <c r="N31" s="14"/>
-      <c r="O31" s="121"/>
+      <c r="O31" s="120"/>
     </row>
     <row r="32" spans="1:15" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
@@ -3336,11 +3345,11 @@
       <c r="L32" s="100"/>
       <c r="M32" s="106"/>
       <c r="N32" s="15"/>
-      <c r="O32" s="121"/>
+      <c r="O32" s="120"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="126"/>
-      <c r="B33" s="126"/>
+      <c r="A33" s="125"/>
+      <c r="B33" s="125"/>
       <c r="C33" s="76"/>
       <c r="D33" s="76"/>
       <c r="E33" s="76"/>
@@ -3367,8 +3376,8 @@
         <v>56</v>
       </c>
       <c r="F34" s="80"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="130"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="129"/>
       <c r="I34" s="82" t="s">
         <v>57</v>
       </c>
@@ -3379,45 +3388,45 @@
       <c r="N34" s="17"/>
     </row>
     <row r="35" spans="1:14" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="126"/>
-      <c r="B35" s="126"/>
-      <c r="C35" s="130"/>
-      <c r="D35" s="130"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="130"/>
-      <c r="G35" s="130"/>
-      <c r="H35" s="130"/>
-      <c r="I35" s="130"/>
-      <c r="J35" s="130"/>
-      <c r="K35" s="130"/>
-      <c r="L35" s="131"/>
-      <c r="M35" s="121"/>
-      <c r="N35" s="121"/>
+      <c r="A35" s="125"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="129"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="129"/>
+      <c r="K35" s="129"/>
+      <c r="L35" s="130"/>
+      <c r="M35" s="120"/>
+      <c r="N35" s="120"/>
     </row>
     <row r="36" spans="1:14" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="126"/>
+      <c r="A36" s="125"/>
       <c r="B36" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="149" t="s">
+      <c r="C36" s="148" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="150"/>
-      <c r="E36" s="150"/>
-      <c r="F36" s="150"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="150"/>
-      <c r="I36" s="151"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="149"/>
+      <c r="F36" s="149"/>
+      <c r="G36" s="149"/>
+      <c r="H36" s="149"/>
+      <c r="I36" s="150"/>
       <c r="J36" s="85"/>
-      <c r="K36" s="152" t="s">
+      <c r="K36" s="151" t="s">
         <v>60</v>
       </c>
-      <c r="L36" s="153"/>
-      <c r="M36" s="154"/>
+      <c r="L36" s="152"/>
+      <c r="M36" s="153"/>
       <c r="N36" s="18"/>
     </row>
     <row r="37" spans="1:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="126"/>
+      <c r="A37" s="125"/>
       <c r="B37" s="24" t="s">
         <v>61</v>
       </c>
@@ -3441,94 +3450,94 @@
         <v>66</v>
       </c>
       <c r="J37" s="86"/>
-      <c r="K37" s="155" t="s">
+      <c r="K37" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="L37" s="156"/>
+      <c r="L37" s="155"/>
       <c r="M37" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N37" s="121"/>
+      <c r="N37" s="120"/>
     </row>
     <row r="38" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="126"/>
+      <c r="A38" s="125"/>
       <c r="B38" s="19"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="132">
+      <c r="C38" s="119"/>
+      <c r="D38" s="131">
         <f>J15+J16+J17+J18+J19+J23+J27+J26+J28+J24+J25+J29</f>
         <v>0</v>
       </c>
       <c r="E38" s="87"/>
-      <c r="F38" s="133"/>
-      <c r="G38" s="132"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="134"/>
-      <c r="J38" s="135"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="133"/>
+      <c r="J38" s="134"/>
       <c r="K38" s="88"/>
       <c r="L38" s="26"/>
       <c r="M38" s="27"/>
-      <c r="N38" s="121"/>
+      <c r="N38" s="120"/>
     </row>
     <row r="39" spans="1:14" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="126"/>
+      <c r="A39" s="125"/>
       <c r="B39" s="19"/>
-      <c r="C39" s="120"/>
-      <c r="D39" s="136">
+      <c r="C39" s="163"/>
+      <c r="D39" s="135">
         <f>J20+J21</f>
         <v>0</v>
       </c>
       <c r="E39" s="90"/>
-      <c r="F39" s="137"/>
-      <c r="G39" s="136"/>
-      <c r="H39" s="136"/>
-      <c r="I39" s="138"/>
-      <c r="J39" s="135"/>
+      <c r="F39" s="136"/>
+      <c r="G39" s="135"/>
+      <c r="H39" s="135"/>
+      <c r="I39" s="137"/>
+      <c r="J39" s="134"/>
       <c r="K39" s="91"/>
       <c r="L39" s="28"/>
       <c r="M39" s="29"/>
-      <c r="N39" s="121"/>
+      <c r="N39" s="120"/>
     </row>
     <row r="40" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="126"/>
+      <c r="A40" s="125"/>
       <c r="B40" s="25" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="89"/>
-      <c r="D40" s="136"/>
+      <c r="D40" s="135"/>
       <c r="E40" s="92"/>
-      <c r="F40" s="137"/>
-      <c r="G40" s="136"/>
-      <c r="H40" s="136"/>
-      <c r="I40" s="138"/>
-      <c r="J40" s="135"/>
+      <c r="F40" s="136"/>
+      <c r="G40" s="135"/>
+      <c r="H40" s="135"/>
+      <c r="I40" s="137"/>
+      <c r="J40" s="134"/>
       <c r="K40" s="91"/>
       <c r="L40" s="28"/>
       <c r="M40" s="29"/>
-      <c r="N40" s="121"/>
+      <c r="N40" s="120"/>
     </row>
     <row r="41" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="126"/>
+      <c r="A41" s="125"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="139"/>
-      <c r="D41" s="140"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="139"/>
       <c r="E41" s="93"/>
-      <c r="F41" s="141"/>
-      <c r="G41" s="140"/>
-      <c r="H41" s="140"/>
-      <c r="I41" s="142"/>
-      <c r="J41" s="135"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="139"/>
+      <c r="I41" s="141"/>
+      <c r="J41" s="134"/>
       <c r="K41" s="91"/>
       <c r="L41" s="28"/>
       <c r="M41" s="29"/>
-      <c r="N41" s="121"/>
+      <c r="N41" s="120"/>
     </row>
     <row r="42" spans="1:14" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="126"/>
+      <c r="A42" s="125"/>
       <c r="B42" s="23"/>
       <c r="C42" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="143">
+      <c r="D42" s="142">
         <f>D40+D39+D38</f>
         <v>0</v>
       </c>
@@ -3536,39 +3545,39 @@
         <f>D42</f>
         <v>0</v>
       </c>
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="143">
+      <c r="F42" s="143"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="142">
         <f>IF(G42&lt;E42,E42-G42,0)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="145">
+      <c r="I42" s="144">
         <f>IF(G42&gt;E42,G42-E42,0)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="135"/>
+      <c r="J42" s="134"/>
       <c r="K42" s="101"/>
       <c r="L42" s="102"/>
       <c r="M42" s="103"/>
-      <c r="N42" s="121"/>
+      <c r="N42" s="120"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="126"/>
+      <c r="A43" s="125"/>
       <c r="B43" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="130"/>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130"/>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="146"/>
-      <c r="J43" s="146"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="131"/>
-      <c r="M43" s="121"/>
-      <c r="N43" s="121"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="K43" s="129"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="120"/>
+      <c r="N43" s="120"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0"/>

</xml_diff>